<commit_message>
added calculation for a 0,75 R to see how long numbers need to fall <1000
</commit_message>
<xml_diff>
--- a/src/CoronaDataHelper/CoronaDataHelper/res/Exp-Example.xlsx
+++ b/src/CoronaDataHelper/CoronaDataHelper/res/Exp-Example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christoph\Documents\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\coronaDataHelper\src\CoronaDataHelper\CoronaDataHelper\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05AD121D-4F8B-42B4-8065-F3CB69B26DFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36CC646-F99B-46E2-8D86-9E675B7F8953}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{233D17F4-F1C4-4491-B917-535F87026414}"/>
   </bookViews>
@@ -450,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109AD448-D389-4730-901F-F301F14041E5}">
-  <dimension ref="A1:AB17"/>
+  <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" activeCellId="9" sqref="X3:AB3 Y4 X4 W4 V4 U4 T4 S4 R4 Q4"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2271,8 +2271,116 @@
         <v>444089209850.06873</v>
       </c>
     </row>
-    <row r="17" spans="28:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB17" s="6"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.75</v>
+      </c>
+      <c r="B19" s="13">
+        <v>20000</v>
+      </c>
+      <c r="C19" s="14">
+        <f>B19*$A$19</f>
+        <v>15000</v>
+      </c>
+      <c r="D19" s="14">
+        <f t="shared" ref="D19:AA19" si="17">C19*$A$19</f>
+        <v>11250</v>
+      </c>
+      <c r="E19" s="14">
+        <f t="shared" si="17"/>
+        <v>8437.5</v>
+      </c>
+      <c r="F19" s="14">
+        <f t="shared" si="17"/>
+        <v>6328.125</v>
+      </c>
+      <c r="G19" s="14">
+        <f t="shared" si="17"/>
+        <v>4746.09375</v>
+      </c>
+      <c r="H19" s="14">
+        <f t="shared" si="17"/>
+        <v>3559.5703125</v>
+      </c>
+      <c r="I19" s="14">
+        <f t="shared" si="17"/>
+        <v>2669.677734375</v>
+      </c>
+      <c r="J19" s="14">
+        <f t="shared" si="17"/>
+        <v>2002.25830078125</v>
+      </c>
+      <c r="K19" s="14">
+        <f t="shared" si="17"/>
+        <v>1501.6937255859375</v>
+      </c>
+      <c r="L19" s="14">
+        <f t="shared" si="17"/>
+        <v>1126.2702941894531</v>
+      </c>
+      <c r="M19" s="14">
+        <f t="shared" si="17"/>
+        <v>844.70272064208984</v>
+      </c>
+      <c r="N19" s="14">
+        <f t="shared" si="17"/>
+        <v>633.52704048156738</v>
+      </c>
+      <c r="O19" s="14">
+        <f t="shared" si="17"/>
+        <v>475.14528036117554</v>
+      </c>
+      <c r="P19" s="14">
+        <f t="shared" si="17"/>
+        <v>356.35896027088165</v>
+      </c>
+      <c r="Q19" s="14">
+        <f t="shared" si="17"/>
+        <v>267.26922020316124</v>
+      </c>
+      <c r="R19" s="14">
+        <f t="shared" si="17"/>
+        <v>200.45191515237093</v>
+      </c>
+      <c r="S19" s="14">
+        <f t="shared" si="17"/>
+        <v>150.3389363642782</v>
+      </c>
+      <c r="T19" s="14">
+        <f t="shared" si="17"/>
+        <v>112.75420227320865</v>
+      </c>
+      <c r="U19" s="14">
+        <f t="shared" si="17"/>
+        <v>84.565651704906486</v>
+      </c>
+      <c r="V19" s="14">
+        <f t="shared" si="17"/>
+        <v>63.424238778679864</v>
+      </c>
+      <c r="W19" s="14">
+        <f t="shared" si="17"/>
+        <v>47.568179084009898</v>
+      </c>
+      <c r="X19" s="14">
+        <f t="shared" si="17"/>
+        <v>35.676134313007424</v>
+      </c>
+      <c r="Y19" s="14">
+        <f t="shared" si="17"/>
+        <v>26.757100734755568</v>
+      </c>
+      <c r="Z19" s="14">
+        <f t="shared" si="17"/>
+        <v>20.067825551066676</v>
+      </c>
+      <c r="AA19" s="14">
+        <f t="shared" si="17"/>
+        <v>15.050869163300007</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>